<commit_message>
fix alignment of buttons
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung/Zeitaufzeichnung.xlsx
+++ b/Zeitaufzeichnung/Zeitaufzeichnung.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -66,6 +66,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -162,33 +163,33 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -220,7 +221,7 @@
       </c>
       <c r="E3" s="3" t="n">
         <f aca="false">SUM(D3:D50)</f>
-        <v>0.333333333333333</v>
+        <v>0.437500000000001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -245,8 +246,13 @@
       <c r="B5" s="3" t="n">
         <v>0.4375</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="3" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <f aca="false">C5-B5</f>
+        <v>0.104166666666667</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>

</xml_diff>

<commit_message>
update Zeitaufzeichnung and other stuff
</commit_message>
<xml_diff>
--- a/Zeitaufzeichnung/Zeitaufzeichnung.xlsx
+++ b/Zeitaufzeichnung/Zeitaufzeichnung.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t xml:space="preserve">Romano</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t xml:space="preserve">10.06.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.06.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.06.22</t>
   </si>
 </sst>
 </file>
@@ -189,10 +195,10 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -232,7 +238,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="n">
@@ -247,11 +253,11 @@
       </c>
       <c r="E3" s="3" t="n">
         <f aca="false">SUM(D3:D50)</f>
-        <v>1.95833333333333</v>
+        <v>2.16666666666667</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="n">
@@ -266,7 +272,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2" t="n">
@@ -386,16 +392,34 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <f aca="false">C13-B13</f>
+        <v>0.0833333333333333</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <f aca="false">C14-B14</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
@@ -565,7 +589,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>